<commit_message>
Update local development changes and data files
- Modified Excel input/output data files
- Updated preprocessing modules (fabric combiner, operation limits, sequence)
- Enhanced DAG management and results processing
- Added new Excel data files for reference
</commit_message>
<xml_diff>
--- a/python_engine/data/input/생산계획_db샘플.xlsx
+++ b/python_engine/data/input/생산계획_db샘플.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohyun\OneDrive\바탕 화면\스케줄링\production-scheduling-system(local_updates)\production-scheduling-system\python_engine\data\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kim\OneDrive\바탕 화면\생산계획\스케줄링-0923 (local-updates branch)\python_engine\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1BF6A0-B10F-4C5D-97AF-1C1C22F9B007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7859708B-8AB1-45B9-B7D3-315BA47D5D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="7" xr2:uid="{A1827C79-4B8F-4B8B-B4CA-C1C5AC227E84}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="5" xr2:uid="{A1827C79-4B8F-4B8B-B4CA-C1C5AC227E84}"/>
   </bookViews>
   <sheets>
     <sheet name="order_data" sheetId="3" r:id="rId1"/>
@@ -26,6 +26,9 @@
     <sheet name="machine_allocate" sheetId="12" r:id="rId11"/>
     <sheet name="machine_rest" sheetId="13" r:id="rId12"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">operation_types!$A$1:$D$39</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="168">
   <si>
     <t>한글명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,10 +132,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>공정분류</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>P/O NO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -193,14 +192,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>id_gitem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tx_gitem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>width</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -354,12 +345,6 @@
     <t>C2010, C2260</t>
   </si>
   <si>
-    <t>기계인덱스</t>
-  </si>
-  <si>
-    <t>기계이름</t>
-  </si>
-  <si>
     <t>1호기</t>
   </si>
   <si>
@@ -384,18 +369,6 @@
     <t>51호기</t>
   </si>
   <si>
-    <t>tx_operation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_operation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tx_operation_type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>operation_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -418,30 +391,10 @@
     <t>operation_7</t>
   </si>
   <si>
-    <t>id_machine</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>yield</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>idx_machine</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tx_machine</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기계인덱스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기계명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>long_to_short</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -498,26 +451,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1호기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>26호기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>27호기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id_mixture</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>idx_operation_seq</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -634,6 +571,58 @@
   </si>
   <si>
     <t>type_change_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GitemNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GItemName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROCCODE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROCSEQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROCNAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProcGbn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공정군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>호기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MachineName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MachineIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MachineNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>호기인덱스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>호기코드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -644,7 +633,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,8 +658,24 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -681,6 +686,16 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -721,12 +736,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -750,8 +771,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="나쁨" xfId="2" builtinId="27"/>
+    <cellStyle name="좋음" xfId="1" builtinId="26"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1087,84 +1120,84 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>170</v>
-      </c>
-      <c r="I2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B3" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="C3" s="1">
         <v>31704</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E3" s="1">
         <v>1524</v>
@@ -1182,15 +1215,15 @@
         <v>45798</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1">
         <v>31798</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E4" s="1">
         <v>1524</v>
@@ -1208,15 +1241,15 @@
         <v>45839</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1">
         <v>31800</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E5" s="1">
         <v>1524</v>
@@ -1234,15 +1267,15 @@
         <v>45839</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1">
         <v>31802</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1">
         <v>1524</v>
@@ -1260,15 +1293,15 @@
         <v>45839</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1">
         <v>31864</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E7" s="1">
         <v>508</v>
@@ -1286,15 +1319,15 @@
         <v>45805</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1">
         <v>31864</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E8" s="1">
         <v>609</v>
@@ -1312,15 +1345,15 @@
         <v>45805</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1">
         <v>31864</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E9" s="1">
         <v>914</v>
@@ -1338,15 +1371,15 @@
         <v>45805</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1">
         <v>31864</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E10" s="1">
         <v>1016</v>
@@ -1364,15 +1397,15 @@
         <v>45805</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1">
         <v>31540</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E11" s="1">
         <v>508</v>
@@ -1390,15 +1423,15 @@
         <v>45805</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1">
         <v>31540</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E12" s="1">
         <v>609</v>
@@ -1416,15 +1449,15 @@
         <v>45805</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1">
         <v>31540</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E13" s="1">
         <v>914</v>
@@ -1442,15 +1475,15 @@
         <v>45805</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1">
         <v>31540</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E14" s="1">
         <v>1016</v>
@@ -1479,37 +1512,37 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>110</v>
+      <c r="B2" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1523,35 +1556,35 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:C2"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>110</v>
+      <c r="B2" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1562,46 +1595,55 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001249FE-5691-4472-B329-BDC14B9A31F7}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C1" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>110</v>
+      <c r="B2" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" t="s">
-        <v>169</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="12">
+        <v>45792</v>
+      </c>
+      <c r="D3" s="12">
+        <v>45793</v>
       </c>
     </row>
   </sheetData>
@@ -1615,16 +1657,16 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1632,7 +1674,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -1659,15 +1701,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>100</v>
+      <c r="B2" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>157</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -1694,12 +1736,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>31540</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>63</v>
+      <c r="C3" s="1">
+        <v>20300</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1">
@@ -1711,12 +1753,12 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>31540</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>65</v>
+      <c r="C4" s="1">
+        <v>20700</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1729,12 +1771,12 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>31704</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>67</v>
+      <c r="C5" s="1">
+        <v>23311</v>
       </c>
       <c r="D5" s="1">
         <v>10</v>
@@ -1747,12 +1789,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>31704</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>69</v>
+      <c r="C6" s="1">
+        <v>12400</v>
       </c>
       <c r="D6" s="1">
         <v>10</v>
@@ -1765,12 +1807,12 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>31798</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>73</v>
+      <c r="C7" s="1">
+        <v>20706</v>
       </c>
       <c r="D7" s="1">
         <v>8.3000000000000007</v>
@@ -1785,12 +1827,12 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>31798</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>71</v>
+      <c r="C8" s="1">
+        <v>20902</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1803,12 +1845,12 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>31798</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>77</v>
+      <c r="C9" s="1">
+        <v>20906</v>
       </c>
       <c r="D9" s="1">
         <v>18</v>
@@ -1823,12 +1865,12 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>31798</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>75</v>
+      <c r="C10" s="1">
+        <v>20500</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1843,12 +1885,12 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>31800</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>73</v>
+      <c r="C11" s="1">
+        <v>20706</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1861,12 +1903,12 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>31800</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>71</v>
+      <c r="C12" s="1">
+        <v>20902</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1879,12 +1921,12 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>31800</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>77</v>
+      <c r="C13" s="1">
+        <v>20906</v>
       </c>
       <c r="D13" s="1">
         <v>23.1</v>
@@ -1899,12 +1941,12 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>31800</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>75</v>
+      <c r="C14" s="1">
+        <v>20500</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1917,12 +1959,12 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>31802</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>73</v>
+      <c r="C15" s="1">
+        <v>20706</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1935,12 +1977,12 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>31802</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>71</v>
+      <c r="C16" s="1">
+        <v>20902</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1953,12 +1995,12 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>31802</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>77</v>
+      <c r="C17" s="1">
+        <v>20906</v>
       </c>
       <c r="D17" s="1">
         <v>22.1</v>
@@ -1973,12 +2015,12 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>31802</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>75</v>
+      <c r="C18" s="1">
+        <v>20500</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1991,12 +2033,12 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>31864</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>63</v>
+      <c r="C19" s="1">
+        <v>20300</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -2009,12 +2051,12 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>31864</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>65</v>
+      <c r="C20" s="1">
+        <v>20700</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2027,7 +2069,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D21" s="1"/>
     </row>
   </sheetData>
@@ -2041,16 +2083,17 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2061,431 +2104,432 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B2" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>20920</v>
       </c>
       <c r="C3" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>23312</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>23320</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>23315</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>23316</v>
       </c>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>20703</v>
       </c>
       <c r="C8" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="D8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>20711</v>
       </c>
       <c r="C9" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>20708</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>20710</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>21000</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="D12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>20900</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="D13" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>20702</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="D14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>20713</v>
       </c>
       <c r="C15" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="D15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>20706</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>20714</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>20704</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="D18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>20707</v>
       </c>
       <c r="C19" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>12400</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>20709</v>
       </c>
       <c r="C21" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D21" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>20705</v>
       </c>
       <c r="C22" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>20700</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>20601</v>
       </c>
       <c r="C24" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="D24" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.4">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>20904</v>
       </c>
       <c r="C25" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.4">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>23119</v>
       </c>
       <c r="C26" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.4">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>23118</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.4">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>20902</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.4">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>20300</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>20400</v>
       </c>
       <c r="C30" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="D30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>23311</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>23100</v>
       </c>
       <c r="C32" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="D32" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>23200</v>
       </c>
       <c r="C33" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="D33" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>23300</v>
       </c>
       <c r="C34" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="D34" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>20500</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D35" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>20600</v>
       </c>
       <c r="C36" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="D36" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>80013</v>
       </c>
       <c r="C37" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="D37" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>25005</v>
       </c>
       <c r="C38" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="D38" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>20906</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D39" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D39" xr:uid="{1EC8C71B-5C87-488F-AE65-B3C4E5C89605}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2496,17 +2540,17 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2514,142 +2558,142 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>39</v>
+      <c r="B2" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="I2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>31798</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>31800</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>31802</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>31540</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>31864</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>31704</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2665,18 +2709,18 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.19921875" customWidth="1"/>
-    <col min="5" max="5" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" customWidth="1"/>
+    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2690,33 +2734,33 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>100</v>
+      <c r="B2" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>159</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+        <v>117</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>31540</v>
       </c>
@@ -2724,16 +2768,16 @@
         <v>20300</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>31540</v>
       </c>
@@ -2741,16 +2785,16 @@
         <v>20700</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>31704</v>
       </c>
@@ -2758,16 +2802,16 @@
         <v>23311</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>31704</v>
       </c>
@@ -2775,10 +2819,10 @@
         <v>12400</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
@@ -2789,7 +2833,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>31798</v>
       </c>
@@ -2797,10 +2841,10 @@
         <v>20902</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -2811,7 +2855,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>31798</v>
       </c>
@@ -2819,10 +2863,10 @@
         <v>20706</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F8" s="1">
         <v>2</v>
@@ -2833,7 +2877,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>31798</v>
       </c>
@@ -2841,10 +2885,10 @@
         <v>20500</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F9" s="1">
         <v>3</v>
@@ -2855,7 +2899,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>31798</v>
       </c>
@@ -2863,10 +2907,10 @@
         <v>20906</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F10" s="1">
         <v>4</v>
@@ -2877,7 +2921,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>31800</v>
       </c>
@@ -2885,10 +2929,10 @@
         <v>20902</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
@@ -2899,7 +2943,7 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>31800</v>
       </c>
@@ -2907,10 +2951,10 @@
         <v>20706</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F12" s="1">
         <v>2</v>
@@ -2921,7 +2965,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>31800</v>
       </c>
@@ -2929,10 +2973,10 @@
         <v>20500</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F13" s="1">
         <v>3</v>
@@ -2943,7 +2987,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>31800</v>
       </c>
@@ -2951,10 +2995,10 @@
         <v>20906</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F14" s="1">
         <v>4</v>
@@ -2965,7 +3009,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>31802</v>
       </c>
@@ -2973,10 +3017,10 @@
         <v>20902</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
@@ -2987,7 +3031,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>31802</v>
       </c>
@@ -2995,10 +3039,10 @@
         <v>20706</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F16" s="1">
         <v>2</v>
@@ -3009,7 +3053,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>31802</v>
       </c>
@@ -3017,10 +3061,10 @@
         <v>20500</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1">
         <v>3</v>
@@ -3031,7 +3075,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>31802</v>
       </c>
@@ -3039,10 +3083,10 @@
         <v>20906</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F18" s="1">
         <v>4</v>
@@ -3053,7 +3097,7 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>31864</v>
       </c>
@@ -3061,10 +3105,10 @@
         <v>20300</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -3075,7 +3119,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>31864</v>
       </c>
@@ -3083,10 +3127,10 @@
         <v>20700</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F20" s="1">
         <v>2</v>
@@ -3107,18 +3151,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4CC067-65AC-46E7-AC80-D6652B1480A8}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.19921875" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3129,35 +3173,35 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" t="s">
-        <v>110</v>
+      <c r="B2" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>31540</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -3166,12 +3210,12 @@
         <v>0.98840000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>31540</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -3180,12 +3224,12 @@
         <v>0.99129999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>31704</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -3194,12 +3238,12 @@
         <v>0.99549999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>31704</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
@@ -3208,26 +3252,26 @@
         <v>0.99099999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>31798</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E7" s="1">
         <v>0.97199999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>31798</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
@@ -3236,26 +3280,26 @@
         <v>0.98959999999999992</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>31798</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E9" s="1">
         <v>0.98699999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>31798</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -3264,26 +3308,26 @@
         <v>0.9778</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>31800</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E11" s="1">
         <v>0.97640000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>31800</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
@@ -3292,12 +3336,12 @@
         <v>0.99159999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>31800</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>12</v>
@@ -3306,12 +3350,12 @@
         <v>0.98470000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>31800</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
@@ -3320,26 +3364,26 @@
         <v>0.97840000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>31802</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E15" s="1">
         <v>0.98109999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>31802</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>12</v>
@@ -3348,12 +3392,12 @@
         <v>0.99040000000000006</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>31802</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>12</v>
@@ -3362,12 +3406,12 @@
         <v>0.9887999999999999</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>31802</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
@@ -3376,12 +3420,12 @@
         <v>0.9779000000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>31864</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>10</v>
@@ -3390,12 +3434,12 @@
         <v>0.9887999999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>31864</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>12</v>
@@ -3415,45 +3459,46 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>162</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>110</v>
+      <c r="B2" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+        <v>164</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
@@ -3461,10 +3506,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -3472,10 +3517,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
@@ -3483,10 +3528,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
@@ -3494,10 +3539,10 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
@@ -3505,10 +3550,10 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3516,10 +3561,10 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
@@ -3527,10 +3572,10 @@
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
@@ -3538,7 +3583,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3551,447 +3596,447 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143E237E-3FF7-4017-8B40-58D2CFFA5646}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D3" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D4" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D5" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D6" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D7" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D8" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D9" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D10" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D11" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D12" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D13" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D14" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D15" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D16" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D17" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D18" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D19" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D20" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D21" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D22" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D23" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D24" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D25" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D26" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D27" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D28" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D29" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D30" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D31" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D32" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D33" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D34" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D35" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D36" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D37" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D38" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D39" s="7">
         <v>0</v>
@@ -4005,98 +4050,82 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E33BFD4-FF40-4B29-B0EF-2F1F0C4A3874}">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" customWidth="1"/>
+    <col min="3" max="4" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>112</v>
+      <c r="B2" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>130</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>131</v>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>132</v>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R10" t="s">
-        <v>135</v>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q10" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>